<commit_message>
added select domain field and clear selection feature with null field validation
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4800" yWindow="4035" windowWidth="15840" windowHeight="10020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -415,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -426,46 +426,121 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>opportunities</t>
+          <t>sgfdgasd</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>अवसर</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>45187.51788336805</v>
+          <t>dfgfd</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>45187.69875416667</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Everything you do in Microsoft Excel, can be automated with Python. So why not use the power of Python and make your life easy. You can make intelligent and thinking Excel sheets, bringing the power of logic and thinking of Python to Excel which is usually static, hence bringing flexibility in Excel and a number of opportunities</t>
+          <t xml:space="preserve">hello </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>माइक्रोसॉफ्ट एक्सेल में आप जो कुछ भी करते हैं, उसे पायथन के साथ स्वचालित किया जा सकता है। तो क्यों न पायथन की शक्ति का उपयोग करें और अपने जीवन को आसान बनाएं। आप इंटेलिजेंट और सोच-विचार वाली एक्सेल शीट बना सकते हैं, जिससे पायथन की तर्क और सोच की शक्</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>45187.52298949074</v>
+          <t>hii</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45187.69890496528</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> of opportunities</t>
+          <t xml:space="preserve">hello </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>जिससे एक्सेल</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>45187.64221642302</v>
+          <t>hii</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45187.69913512732</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hii</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45187.69916291667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hii</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>News</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45187.69919403935</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>hii</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Legal</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45187.69921873264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>